<commit_message>
Add import for dishes
</commit_message>
<xml_diff>
--- a/SmartDietAPI/Data/foods.xlsx
+++ b/SmartDietAPI/Data/foods.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FFF\Sem_8\EXE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FFF\Sem_8\EXE\SmartDietAPI\SmartDietAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40442E2E-6517-4ED9-B5B5-2CFBA8C903F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7B7055-B892-4A5C-9776-8FB21E247A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1530" yWindow="730" windowWidth="16990" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thực phẩm" sheetId="2" r:id="rId1"/>

</xml_diff>